<commit_message>
incorporating Emily's 6/9/24 edits and first spansih draft of first three decision tree case studies.
</commit_message>
<xml_diff>
--- a/case-studies/cs1_PE_v1_ANS.xlsx
+++ b/case-studies/cs1_PE_v1_ANS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyleech/Desktop/GitHub/DecisionAnalysis_AshleyLeech/in-class-exercises/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C514BD2D-3DDA-D54E-BD91-7EF3ADCE1F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94DE28C-43D2-6343-997F-7AB262874FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15040" activeTab="2" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33160" windowHeight="23320" activeTab="2" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="3" r:id="rId1"/>
@@ -387,6 +387,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -397,9 +400,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,9 +776,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -816,7 +816,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -922,7 +922,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1064,7 +1064,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>8.0000000000000002E-3</v>
+        <v>0.04</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -1213,7 +1213,7 @@
   <dimension ref="C1:R53"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,7 +1286,7 @@
     <row r="5" spans="6:18" x14ac:dyDescent="0.2">
       <c r="L5" s="8">
         <f>p_fatal_recurrent_pe_with_ac</f>
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="5"/>
@@ -1329,7 +1329,7 @@
         <v>27</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="L12" s="23"/>
+      <c r="L12" s="24"/>
       <c r="M12" s="6"/>
       <c r="N12" s="15" t="s">
         <v>30</v>
@@ -1350,7 +1350,7 @@
       <c r="I13" s="7"/>
       <c r="L13" s="8">
         <f>1-p_fatal_recurrent_pe_with_ac</f>
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="5"/>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="L18" s="8">
         <f>p_fatal_bleed_with_ac</f>
-        <v>8.0000000000000002E-3</v>
+        <v>0.04</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="5"/>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="19" spans="3:18" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F19" s="7"/>
-      <c r="I19" s="23"/>
+      <c r="I19" s="24"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.2">
@@ -1436,7 +1436,7 @@
     </row>
     <row r="24" spans="3:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F24" s="7"/>
-      <c r="L24" s="23"/>
+      <c r="L24" s="24"/>
       <c r="M24" s="6"/>
       <c r="N24" s="15" t="s">
         <v>23</v>
@@ -1451,10 +1451,10 @@
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="F25" s="27"/>
+      <c r="F25" s="23"/>
       <c r="L25" s="8">
         <f>1-p_fatal_bleed_with_ac</f>
-        <v>0.99199999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="N25" s="14"/>
       <c r="P25" s="14"/>
@@ -1462,7 +1462,7 @@
       <c r="R25" s="14"/>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="F26" s="27"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="3:18" x14ac:dyDescent="0.2">
       <c r="F27" s="9"/>
@@ -1473,12 +1473,12 @@
       </c>
       <c r="D28" s="6"/>
       <c r="F28" s="7"/>
-      <c r="L28" s="26"/>
+      <c r="L28" s="27"/>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C29" s="22"/>
       <c r="F29" s="7"/>
-      <c r="L29" s="26"/>
+      <c r="L29" s="27"/>
       <c r="N29" s="14"/>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.2">
@@ -1555,7 +1555,7 @@
         <v>28</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="L39" s="23"/>
+      <c r="L39" s="24"/>
       <c r="M39" s="6"/>
       <c r="N39" s="15" t="s">
         <v>26</v>
@@ -1583,7 +1583,7 @@
       <c r="R40" s="14"/>
     </row>
     <row r="41" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="F41" s="23"/>
+      <c r="F41" s="24"/>
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="6:18" x14ac:dyDescent="0.2">
@@ -1592,11 +1592,11 @@
     </row>
     <row r="43" spans="6:18" x14ac:dyDescent="0.2">
       <c r="I43" s="7"/>
-      <c r="L43" s="24"/>
+      <c r="L43" s="25"/>
     </row>
     <row r="44" spans="6:18" x14ac:dyDescent="0.2">
       <c r="I44" s="7"/>
-      <c r="L44" s="24"/>
+      <c r="L44" s="25"/>
       <c r="N44" s="14"/>
     </row>
     <row r="45" spans="6:18" x14ac:dyDescent="0.2">
@@ -1606,8 +1606,8 @@
       <c r="N45" s="14"/>
     </row>
     <row r="46" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="23"/>
-      <c r="L46" s="24" t="s">
+      <c r="I46" s="24"/>
+      <c r="L46" s="25" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
-      <c r="L47" s="25"/>
+      <c r="L47" s="26"/>
       <c r="M47" s="6"/>
       <c r="N47" s="15" t="s">
         <v>25</v>
@@ -1639,23 +1639,13 @@
       <c r="R48" s="14"/>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F52" s="24"/>
+      <c r="F52" s="25"/>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F53" s="24"/>
+      <c r="F53" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L43:L44"/>
     <mergeCell ref="I45:I46"/>
     <mergeCell ref="L46:L47"/>
     <mergeCell ref="F52:F53"/>
@@ -1664,6 +1654,16 @@
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="L31:L32"/>
     <mergeCell ref="F39:F41"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L23:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="197" zoomScaleNormal="197" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,15 +1706,15 @@
       </c>
       <c r="C3" s="17">
         <f>'Decision Tree'!P4*'Decision Tree'!L5*'Decision Tree'!I10+'Decision Tree'!P12*'Decision Tree'!L13*'Decision Tree'!I10+'Decision Tree'!P17*'Decision Tree'!L18*'Decision Tree'!I20+'Decision Tree'!P24*'Decision Tree'!L25*'Decision Tree'!I20</f>
-        <v>2033.8000000000002</v>
+        <v>2369</v>
       </c>
       <c r="D3" s="16">
         <f>'Decision Tree'!R4*'Decision Tree'!L5*'Decision Tree'!I10+'Decision Tree'!R12*'Decision Tree'!L13*'Decision Tree'!I10+'Decision Tree'!R17*'Decision Tree'!L18*'Decision Tree'!I20+'Decision Tree'!R24*'Decision Tree'!L25*'Decision Tree'!I20</f>
-        <v>0.99161999999999995</v>
+        <v>0.95810000000000006</v>
       </c>
       <c r="E3" s="18">
         <f>N_pop*(1-D3)</f>
-        <v>838.00000000000546</v>
+        <v>4189.9999999999936</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>